<commit_message>
new data with date occurred
</commit_message>
<xml_diff>
--- a/data/closure_reasons.xlsx
+++ b/data/closure_reasons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/Fraternities and Sexual Assault/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/fraternities/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDFFB74-A71A-8242-A122-AA9692E8950D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEC800E-8F14-2C46-87CC-CC38DF3B8627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36420" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{32D34035-B355-F642-B92E-087571986459}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{32D34035-B355-F642-B92E-087571986459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -921,9 +921,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FC9523-3149-8C4E-9C5D-0B73B2D4C82B}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,6 +931,8 @@
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="3" width="130" style="5" customWidth="1"/>
     <col min="4" max="4" width="29.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1298,9 +1300,7 @@
       <c r="D17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="4">
-        <v>43219</v>
-      </c>
+      <c r="E17" s="4"/>
       <c r="F17" s="4">
         <v>43339</v>
       </c>

</xml_diff>

<commit_message>
update to paper 290 april
</commit_message>
<xml_diff>
--- a/data/closure_reasons.xlsx
+++ b/data/closure_reasons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/fraternities/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C31B99-AD0C-9A40-9C5A-42F20E297AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B39781-B7B1-FE46-A90F-80BF691614F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35980" yWindow="500" windowWidth="38080" windowHeight="21100" xr2:uid="{32D34035-B355-F642-B92E-087571986459}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{32D34035-B355-F642-B92E-087571986459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="130">
   <si>
     <t>University</t>
   </si>
@@ -141,9 +141,6 @@
     <t>University of Pittsburgh-Pittsburgh Campus</t>
   </si>
   <si>
-    <t>University of Vermont</t>
-  </si>
-  <si>
     <t>University of Virginia-Main Campus</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
   </si>
   <si>
     <t xml:space="preserve">With three UNM fraternities already in “emergency suspension” following allegations of hazing or alcohol policy violations, administrators have ordered a two-month halt to most social events within the university’s larger Greek system.” </t>
-  </si>
-  <si>
-    <t>the university continues its investigation into the February death of first-year student Connor Gage.</t>
   </si>
   <si>
     <t>The wrongs described in Rolling Stone are appalling and have caused all of us to reexamine our responsibility to this community. Rape is an abhorrent crime that has no place in the world, let alone on the campuses and grounds of our nation’s colleges and universities. We know, and have felt very powerfully this week, that we are better than we have been described, and that we have a responsibility to live our tradition of honor every day, and as importantly every night.</t>
@@ -333,9 +327,6 @@
     <t>A serious alcohol incident involving members and non-members of one of the fraternities.</t>
   </si>
   <si>
-    <t>Death of Connor Gage.</t>
-  </si>
-  <si>
     <t>Rolling Stone article describing the fraternity culture at the school.</t>
   </si>
   <si>
@@ -460,7 +451,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -543,12 +534,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
       <color rgb="FF111111"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -574,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -610,9 +595,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -930,11 +912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FC9523-3149-8C4E-9C5D-0B73B2D4C82B}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,25 +933,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="44" x14ac:dyDescent="0.25">
@@ -977,10 +959,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D2" s="3">
         <v>42776</v>
@@ -989,9 +971,9 @@
         <v>42787</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="16">
+        <v>92</v>
+      </c>
+      <c r="G2" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1000,46 +982,46 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="3">
         <v>43032</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G3" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E4" s="3">
         <v>42017</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3">
         <v>43198</v>
@@ -1048,9 +1030,9 @@
         <v>43207</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" s="16">
+        <v>102</v>
+      </c>
+      <c r="G5" s="15">
         <v>2</v>
       </c>
     </row>
@@ -1059,10 +1041,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D6" s="3">
         <v>43127</v>
@@ -1071,37 +1053,37 @@
         <v>43129</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G6" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:8" ht="96" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E7" s="3">
         <v>42612</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" s="16"/>
+        <v>127</v>
+      </c>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D8" s="3">
         <v>42029</v>
@@ -1110,9 +1092,9 @@
         <v>42032</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" s="16">
+        <v>92</v>
+      </c>
+      <c r="G8" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1121,10 +1103,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D9" s="3">
         <v>41945</v>
@@ -1133,9 +1115,9 @@
         <v>41946</v>
       </c>
       <c r="F9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" s="16">
+        <v>92</v>
+      </c>
+      <c r="G9" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1144,46 +1126,46 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E10" s="3">
         <v>43067</v>
       </c>
       <c r="F10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E11" s="3">
         <v>43101</v>
       </c>
       <c r="F11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G11" s="16"/>
+        <v>127</v>
+      </c>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D12" s="3">
         <v>43042</v>
@@ -1192,9 +1174,9 @@
         <v>43045</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
-      </c>
-      <c r="G12" s="16">
+        <v>93</v>
+      </c>
+      <c r="G12" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1203,28 +1185,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E13" s="3">
         <v>43066</v>
       </c>
       <c r="F13" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" s="16"/>
+        <v>127</v>
+      </c>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D14" s="3">
         <v>42992</v>
@@ -1233,9 +1215,9 @@
         <v>42992</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="16">
+        <v>93</v>
+      </c>
+      <c r="G14" s="15">
         <v>2</v>
       </c>
     </row>
@@ -1244,71 +1226,71 @@
         <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3">
         <v>43027</v>
       </c>
       <c r="F15" t="s">
-        <v>130</v>
-      </c>
-      <c r="G15" s="16"/>
+        <v>127</v>
+      </c>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E16" s="3">
         <v>43164</v>
       </c>
       <c r="F16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G16" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7" ht="216" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E17" s="3">
         <v>43349</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
-      </c>
-      <c r="G17" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3">
         <v>43339</v>
       </c>
       <c r="F18" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18" s="16">
+        <v>127</v>
+      </c>
+      <c r="G18" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1317,10 +1299,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D19" s="3">
         <v>43179</v>
@@ -1329,99 +1311,99 @@
         <v>43179</v>
       </c>
       <c r="F19" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E20" s="3">
         <v>43055</v>
       </c>
       <c r="F20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" ht="96" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E21" s="3">
         <v>43741</v>
       </c>
       <c r="F21" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E22" s="3">
         <v>42787</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E23" s="3">
         <v>42100</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E24" s="3">
         <v>41968</v>
       </c>
       <c r="F24" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="G24" s="15"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -1429,25 +1411,25 @@
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E25" s="3">
         <v>43168</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D26" s="3">
         <v>43776</v>
@@ -1456,9 +1438,9 @@
         <v>43778</v>
       </c>
       <c r="F26" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="16">
+        <v>93</v>
+      </c>
+      <c r="G26" s="15">
         <v>3</v>
       </c>
     </row>
@@ -1467,28 +1449,28 @@
         <v>22</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E27" s="3">
         <v>43786</v>
       </c>
       <c r="F27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G27" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G27" s="15"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" s="3">
         <v>43052</v>
@@ -1497,9 +1479,9 @@
         <v>43053</v>
       </c>
       <c r="F28" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="16">
+        <v>93</v>
+      </c>
+      <c r="G28" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1508,36 +1490,36 @@
         <v>24</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E29" s="3">
         <v>42690</v>
       </c>
       <c r="F29" t="s">
-        <v>105</v>
-      </c>
-      <c r="G29" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G29" s="15"/>
     </row>
     <row r="30" spans="1:7" ht="96" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E30" s="3">
         <v>43567</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
-      </c>
-      <c r="G30" s="16">
+        <v>93</v>
+      </c>
+      <c r="G30" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1546,64 +1528,64 @@
         <v>26</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E31" s="3">
         <v>42659</v>
       </c>
       <c r="F31" t="s">
-        <v>95</v>
-      </c>
-      <c r="G31" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="G31" s="15"/>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E32" s="3">
         <v>43108</v>
       </c>
       <c r="F32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G32" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G32" s="15"/>
     </row>
     <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E33" s="3">
         <v>43081</v>
       </c>
       <c r="F33" t="s">
-        <v>130</v>
-      </c>
-      <c r="G33" s="16"/>
+        <v>127</v>
+      </c>
+      <c r="G33" s="15"/>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D34" s="3">
         <v>42855</v>
@@ -1612,9 +1594,9 @@
         <v>42856</v>
       </c>
       <c r="F34" t="s">
-        <v>96</v>
-      </c>
-      <c r="G34" s="16">
+        <v>93</v>
+      </c>
+      <c r="G34" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1623,82 +1605,82 @@
         <v>30</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E35" s="3">
         <v>43171</v>
       </c>
       <c r="F35" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G35" s="15"/>
     </row>
     <row r="36" spans="1:7" ht="105" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E36" s="3">
         <v>43048</v>
       </c>
       <c r="F36" t="s">
-        <v>95</v>
-      </c>
-      <c r="G36" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="G36" s="15"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E37" s="3">
         <v>43165</v>
       </c>
       <c r="F37" t="s">
-        <v>105</v>
-      </c>
-      <c r="G37" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G37" s="15"/>
     </row>
     <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E38" s="3">
         <v>43077</v>
       </c>
       <c r="F38" t="s">
-        <v>105</v>
-      </c>
-      <c r="G38" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G38" s="15"/>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D39" s="3">
         <v>43118</v>
@@ -1707,138 +1689,115 @@
         <v>43119</v>
       </c>
       <c r="F39" t="s">
-        <v>105</v>
-      </c>
-      <c r="G39" s="16">
+        <v>102</v>
+      </c>
+      <c r="G39" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="42" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:7" ht="168" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="3">
+        <v>41962</v>
+      </c>
+      <c r="E40" s="3">
+        <v>41965</v>
+      </c>
+      <c r="F40" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="3">
-        <v>43498</v>
-      </c>
-      <c r="E40" s="3">
-        <v>43501</v>
-      </c>
-      <c r="F40" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" s="16">
+      <c r="G40" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="168" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="21" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="15" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3">
+        <v>42681</v>
+      </c>
+      <c r="F41" t="s">
+        <v>127</v>
+      </c>
+      <c r="G41" s="15"/>
+    </row>
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="3">
+        <v>43781</v>
+      </c>
+      <c r="E42" s="3">
+        <v>43783</v>
+      </c>
+      <c r="F42" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="3">
-        <v>41962</v>
-      </c>
-      <c r="E41" s="3">
-        <v>41965</v>
-      </c>
-      <c r="F41" t="s">
-        <v>95</v>
-      </c>
-      <c r="G41" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="21" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3">
-        <v>42681</v>
-      </c>
-      <c r="F42" t="s">
-        <v>130</v>
-      </c>
-      <c r="G42" s="16"/>
-    </row>
-    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="G42" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="3">
+        <v>41955</v>
+      </c>
+      <c r="E43" s="3">
+        <v>41956</v>
+      </c>
+      <c r="F43" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="3">
-        <v>43781</v>
-      </c>
-      <c r="E43" s="3">
-        <v>43783</v>
-      </c>
-      <c r="F43" t="s">
-        <v>96</v>
-      </c>
-      <c r="G43" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" s="3">
-        <v>41955</v>
+      <c r="C44" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="E44" s="3">
-        <v>41956</v>
+        <v>43145</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
-      </c>
-      <c r="G44" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E45" s="3">
-        <v>43145</v>
-      </c>
-      <c r="F45" t="s">
-        <v>105</v>
-      </c>
-      <c r="G45" s="16"/>
+        <v>102</v>
+      </c>
+      <c r="G44" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>